<commit_message>
now can upload train data log file
</commit_message>
<xml_diff>
--- a/backend/training/data/yo_H_train_spacy.xlsx
+++ b/backend/training/data/yo_H_train_spacy.xlsx
@@ -921,7 +921,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PronType=Rel Person=3|Number=Sing|VerbForm=Tns  POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve"> PronType=Rel Person=3|Number=Sing|VerbForm=Tns  Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -933,7 +933,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog   POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve"> PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog   Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -945,7 +945,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog    POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve"> PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog    Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -957,7 +957,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PronType=Rel   VerbForm=Prog  POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve"> PronType=Rel   VerbForm=Prog  Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -969,7 +969,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t xml:space="preserve">  PronType=Rel  VerbForm=Prog    POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve">  PronType=Rel  VerbForm=Prog    Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -981,7 +981,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PronType=Rel    PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog    PronType=Rel Person=3|Number=Sing|VerbForm=Tns   Person=3|Number=Sing|Case=Gen POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve"> PronType=Rel    PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog    PronType=Rel Person=3|Number=Sing|VerbForm=Tns   Person=3|Number=Sing|Case=Gen Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -993,7 +993,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PronType=Rel    Case=Loc  Person=3|Number=Sing|Case=Gen POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve"> PronType=Rel    Case=Loc  Person=3|Number=Sing|Case=Gen Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -1005,7 +1005,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t xml:space="preserve">  PronType=Rel   VerbForm=Prog  Case=Loc  POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve">  PronType=Rel   VerbForm=Prog  Case=Loc  Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -1017,7 +1017,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t xml:space="preserve">  PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog    POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve">  PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog    Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -1029,7 +1029,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t xml:space="preserve">  PronType=Rel   VerbForm=Prog  POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve">  PronType=Rel   VerbForm=Prog  Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -1041,7 +1041,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t xml:space="preserve">  PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog    POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve">  PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog    Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -1053,7 +1053,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t xml:space="preserve">  PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog    POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve">  PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog    Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -1065,7 +1065,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t xml:space="preserve">  PronType=Rel   VerbForm=Prog  POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve">  PronType=Rel   VerbForm=Prog  Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -1077,7 +1077,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t xml:space="preserve">  PronType=Rel   VerbForm=Prog     POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve">  PronType=Rel   VerbForm=Prog     Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -1089,7 +1089,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t xml:space="preserve">  PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog    POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve">  PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog    Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -1101,7 +1101,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PronType=Rel   VerbForm=Prog   Person=3|Number=Sing|Case=Gen POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve"> PronType=Rel   VerbForm=Prog   Person=3|Number=Sing|Case=Gen Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -1113,7 +1113,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t xml:space="preserve">  PronType=Rel   VerbForm=Prog  POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve">  PronType=Rel   VerbForm=Prog  Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -1125,7 +1125,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t xml:space="preserve">  PronType=Rel   VerbForm=Prog  Case=Loc  POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve">  PronType=Rel   VerbForm=Prog  Case=Loc  Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -1137,7 +1137,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PronType=Rel    Case=Loc  Person=3|Number=Sing|Case=Gen POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve"> PronType=Rel    Case=Loc  Person=3|Number=Sing|Case=Gen Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -2385,7 +2385,7 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PronType=Rel   Case=Loc  Person=3|Number=Sing|Case=Gen POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve"> PronType=Rel   Case=Loc  Person=3|Number=Sing|Case=Gen Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -2397,7 +2397,7 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t xml:space="preserve">  PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog    POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve">  PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog    Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -2409,7 +2409,7 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t xml:space="preserve">  PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog    POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve">  PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog    Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -2421,7 +2421,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PronType=Rel    Case=Loc  Person=3|Number=Sing|Case=Gen POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve"> PronType=Rel    Case=Loc  Person=3|Number=Sing|Case=Gen Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -2433,7 +2433,7 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PronType=Rel   VerbForm=Prog  Case=Loc  Person=3|Number=Sing|Case=Gen POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve"> PronType=Rel   VerbForm=Prog  Case=Loc  Person=3|Number=Sing|Case=Gen Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -2445,7 +2445,7 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PronType=Rel   VerbForm=Prog    POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve"> PronType=Rel   VerbForm=Prog    Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -2457,7 +2457,7 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog     POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve"> PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog     Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -2469,7 +2469,7 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t xml:space="preserve">  PronType=Rel   VerbForm=Prog  POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve">  PronType=Rel   VerbForm=Prog  Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -2481,7 +2481,7 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t xml:space="preserve">  PronType=Rel  VerbForm=Prog  Case=Loc  POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve">  PronType=Rel  VerbForm=Prog  Case=Loc  Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -2493,7 +2493,7 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t xml:space="preserve">  PronType=Rel   VerbForm=Prog  POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve">  PronType=Rel   VerbForm=Prog  Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -2505,7 +2505,7 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t xml:space="preserve">  PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog    POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve">  PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog    Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -2517,7 +2517,7 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t xml:space="preserve">  PronType=Rel  VerbForm=Prog    POS=Foc|Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve">  PronType=Rel  VerbForm=Prog    Other=Foc|Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -2529,7 +2529,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PronType=Rel   VerbForm=Prog   Person=3|Number=Sing|Case=Gen POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve"> PronType=Rel   VerbForm=Prog   Person=3|Number=Sing|Case=Gen Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -2541,7 +2541,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t xml:space="preserve">  PronType=Rel   VerbForm=Prog  POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve">  PronType=Rel   VerbForm=Prog  Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -3273,7 +3273,7 @@
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog  POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve"> PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog  Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -3285,7 +3285,7 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PronType=Rel Person=3|Number=Sing|VerbForm=Tns  POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve"> PronType=Rel Person=3|Number=Sing|VerbForm=Tns  Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -3297,7 +3297,7 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PronType=Rel|Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog   POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve"> PronType=Rel|Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog   Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -3309,7 +3309,7 @@
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PronType=Rel|Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog    POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve"> PronType=Rel|Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog    Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -3321,7 +3321,7 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t xml:space="preserve">  PronType=Rel  VerbForm=Prog  POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve">  PronType=Rel  VerbForm=Prog  Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -3333,7 +3333,7 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PronType=Rel  VerbForm=Prog    POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve"> PronType=Rel  VerbForm=Prog    Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -3345,7 +3345,7 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PronType=Rel  VerbForm=Prog    POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve"> PronType=Rel  VerbForm=Prog    Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -3357,7 +3357,7 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t xml:space="preserve">  PronType=Rel   VerbForm=Prog  POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve">  PronType=Rel   VerbForm=Prog  Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -3369,7 +3369,7 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PronType=Rel  VerbForm=Prog  Case=Loc  POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve"> PronType=Rel  VerbForm=Prog  Case=Loc  Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -3381,7 +3381,7 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PronType=Rel|Person=3|Number=Sing|VerbForm=Tns      PronType=Rel    Person=3|Number=Sing|Case=Gen POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve"> PronType=Rel|Person=3|Number=Sing|VerbForm=Tns      PronType=Rel    Person=3|Number=Sing|Case=Gen Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -3393,7 +3393,7 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PronType=Rel  VerbForm=Prog  Case=Loc  POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve"> PronType=Rel  VerbForm=Prog  Case=Loc  Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -3405,7 +3405,7 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t xml:space="preserve">  PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog    POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve">  PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog    Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -3417,7 +3417,7 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t xml:space="preserve">  PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog    POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve">  PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog    Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -3429,7 +3429,7 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t xml:space="preserve">  PronType=Rel  VerbForm=Prog  POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve">  PronType=Rel  VerbForm=Prog  Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -3441,7 +3441,7 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog    POS=Foc Person=3|Number=Sing|VerbForm=Tns      PronType=Rel  VerbForm=Prog   PronType=Rel   VerbForm=Prog  POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve"> PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog    Other=Foc Person=3|Number=Sing|VerbForm=Tns      PronType=Rel  VerbForm=Prog   PronType=Rel   VerbForm=Prog  Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -3453,7 +3453,7 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t xml:space="preserve">  PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog    POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve">  PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog    Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -3465,7 +3465,7 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PronType=Rel    Person=3|Number=Sing|Case=Gen POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve"> PronType=Rel    Person=3|Number=Sing|Case=Gen Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -3477,7 +3477,7 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PronType=Rel  VerbForm=Prog   Person=3|Number=Sing|Case=Gen POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve"> PronType=Rel  VerbForm=Prog   Person=3|Number=Sing|Case=Gen Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -3489,7 +3489,7 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t xml:space="preserve">  PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog    POS=Foc Person=3|Number=Sing|VerbForm=Tns      PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog    POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve">  PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog    Other=Foc Person=3|Number=Sing|VerbForm=Tns      PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog    Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -4005,7 +4005,7 @@
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PronType=Rel|Person=3|Number=Sing|VerbForm=Tns    POS=Foc|Person=3|Number=Sing|VerbForm=Tns  </t>
+          <t xml:space="preserve"> PronType=Rel|Person=3|Number=Sing|VerbForm=Tns    Other=Foc|Person=3|Number=Sing|VerbForm=Tns  </t>
         </is>
       </c>
     </row>
@@ -5085,7 +5085,7 @@
       </c>
       <c r="B388" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog  POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve"> PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog  Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -5757,31 +5757,31 @@
       </c>
       <c r="B444" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog  POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve"> PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog  Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
     <row r="445">
       <c r="A445" t="inlineStr">
         <is>
-          <t>Ehoro tí ó ṣubú ni ó pa àwọ̀ dà</t>
+          <t>Ehoro tí ó ṣubú ni ó pa àwọ̀ dà</t>
         </is>
       </c>
       <c r="B445" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PronType=Rel Person=3|Number=Sing|VerbForm=Tns  POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve"> PronType=Rel Person=3|Number=Sing|VerbForm=Tns  Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
     <row r="446">
       <c r="A446" t="inlineStr">
         <is>
-          <t>Bọ́ọ̀lù tí ó ń yí gbirigbiri ni ó pa àwọ̀ dà</t>
+          <t>Bọ́ọ̀lù tí ó ń yí gbirigbiri ni ó pa àwọ̀ dà</t>
         </is>
       </c>
       <c r="B446" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog   POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve"> PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog   Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -5793,7 +5793,7 @@
       </c>
       <c r="B447" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog    POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve"> PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog    Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -5805,7 +5805,7 @@
       </c>
       <c r="B448" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PronType=Rel   VerbForm=Prog  POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve"> PronType=Rel   VerbForm=Prog  Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -5817,19 +5817,19 @@
       </c>
       <c r="B449" t="inlineStr">
         <is>
-          <t xml:space="preserve">  PronType=Rel  VerbForm=Prog    POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve">  PronType=Rel  VerbForm=Prog    Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
     <row r="450">
       <c r="A450" t="inlineStr">
         <is>
-          <t>*Ilé tí adìyẹ àti àgùntàn tí ó ń fò ati àgùntàn tí ó jókòó lórí rẹ̀ ni ó pa àwọ̀ dà</t>
+          <t>Ilé tí adìyẹ àti àgùntàn tí ó ń fò ati àgùntàn tí ó jókòó lórí rẹ̀ ni ó pa àwọ̀ dà</t>
         </is>
       </c>
       <c r="B450" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PronType=Rel    PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog    PronType=Rel Person=3|Number=Sing|VerbForm=Tns   Person=3|Number=Sing|Case=Gen POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve"> PronType=Rel    PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog    PronType=Rel Person=3|Number=Sing|VerbForm=Tns   Person=3|Number=Sing|Case=Gen Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -5841,7 +5841,7 @@
       </c>
       <c r="B451" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PronType=Rel    Case=Loc  Person=3|Number=Sing|Case=Gen POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve"> PronType=Rel    Case=Loc  Person=3|Number=Sing|Case=Gen Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -5853,7 +5853,7 @@
       </c>
       <c r="B452" t="inlineStr">
         <is>
-          <t xml:space="preserve">  PronType=Rel   VerbForm=Prog  Case=Loc  POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve">  PronType=Rel   VerbForm=Prog  Case=Loc  Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -5865,7 +5865,7 @@
       </c>
       <c r="B453" t="inlineStr">
         <is>
-          <t xml:space="preserve">  PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog    POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve">  PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog    Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -5877,7 +5877,7 @@
       </c>
       <c r="B454" t="inlineStr">
         <is>
-          <t xml:space="preserve">  PronType=Rel   VerbForm=Prog  POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve">  PronType=Rel   VerbForm=Prog  Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -5889,7 +5889,7 @@
       </c>
       <c r="B455" t="inlineStr">
         <is>
-          <t xml:space="preserve">  PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog    POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve">  PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog    Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -5901,7 +5901,7 @@
       </c>
       <c r="B456" t="inlineStr">
         <is>
-          <t xml:space="preserve">  PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog    POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve">  PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog    Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -5913,7 +5913,7 @@
       </c>
       <c r="B457" t="inlineStr">
         <is>
-          <t xml:space="preserve">  PronType=Rel   VerbForm=Prog  POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve">  PronType=Rel   VerbForm=Prog  Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -5925,7 +5925,7 @@
       </c>
       <c r="B458" t="inlineStr">
         <is>
-          <t xml:space="preserve">  PronType=Rel   VerbForm=Prog     POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve">  PronType=Rel   VerbForm=Prog     Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -5937,7 +5937,7 @@
       </c>
       <c r="B459" t="inlineStr">
         <is>
-          <t xml:space="preserve">  PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog    POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve">  PronType=Rel Person=3|Number=Sing|VerbForm=Tns VerbForm=Prog    Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -5949,7 +5949,7 @@
       </c>
       <c r="B460" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PronType=Rel   VerbForm=Prog   Person=3|Number=Sing|Case=Gen POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve"> PronType=Rel   VerbForm=Prog   Person=3|Number=Sing|Case=Gen Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -5961,7 +5961,7 @@
       </c>
       <c r="B461" t="inlineStr">
         <is>
-          <t xml:space="preserve">  PronType=Rel   VerbForm=Prog  POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve">  PronType=Rel   VerbForm=Prog  Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -5973,7 +5973,7 @@
       </c>
       <c r="B462" t="inlineStr">
         <is>
-          <t xml:space="preserve">  PronType=Rel   VerbForm=Prog  Case=Loc  POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve">  PronType=Rel   VerbForm=Prog  Case=Loc  Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>
@@ -5985,7 +5985,7 @@
       </c>
       <c r="B463" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PronType=Rel    Case=Loc  Person=3|Number=Sing|Case=Gen POS=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
+          <t xml:space="preserve"> PronType=Rel    Case=Loc  Person=3|Number=Sing|Case=Gen Other=Foc Person=3|Number=Sing|VerbForm=Tns   </t>
         </is>
       </c>
     </row>

</xml_diff>